<commit_message>
inventario negativo e altri fix
</commit_message>
<xml_diff>
--- a/files_utili/fatture.xlsx
+++ b/files_utili/fatture.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,9 +441,24 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>3524</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>65543</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
-          <t>3524</t>
+          <t>321</t>
         </is>
       </c>
     </row>

</xml_diff>